<commit_message>
fixed templates uploaded new kpis and results added basic_block fixed yogurt special block kpis
</commit_message>
<xml_diff>
--- a/Projects/GMIUS/Data/Mexican GMI KPI template v0.2.xlsx
+++ b/Projects/GMIUS/Data/Mexican GMI KPI template v0.2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="117">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -40,6 +40,12 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
+    <t xml:space="preserve">Dependent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dependent Result</t>
+  </si>
+  <si>
     <t xml:space="preserve">Scene Type</t>
   </si>
   <si>
@@ -157,13 +163,13 @@
     <t xml:space="preserve">How many shelves are in the Shells section?</t>
   </si>
   <si>
-    <t xml:space="preserve">Count of Shelves </t>
+    <t xml:space="preserve">Count of Shelves</t>
   </si>
   <si>
     <t xml:space="preserve">How many shelves are in the Beans section?</t>
   </si>
   <si>
-    <t xml:space="preserve">What segment(s) are adjacent to Herdez Taqueria Street Taco Squeezable Sauces? </t>
+    <t xml:space="preserve">What segment(s) are adjacent to Herdez Taqueria Street Taco Squeezable Sauces?</t>
   </si>
   <si>
     <t xml:space="preserve">Adjacency</t>
@@ -229,9 +235,6 @@
     <t xml:space="preserve">presence_kits</t>
   </si>
   <si>
-    <t xml:space="preserve">KPI name</t>
-  </si>
-  <si>
     <t xml:space="preserve">GMI_BRAND</t>
   </si>
   <si>
@@ -335,9 +338,6 @@
   </si>
   <si>
     <t xml:space="preserve">Entity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shelf length</t>
   </si>
   <si>
     <t xml:space="preserve">Less than or Equal to 4 Feet, 4 Feet &gt; and &lt;= 8 Feet, 8 Feet &gt; and &lt;= 12 Feet, 12 Feet &gt; and &lt;= 16 Feet, 16 Feet &gt; and &lt;= 20 Feet, 20 Feet &gt; and &lt;= 24 Feet, 24 Feet &gt; and &lt;= 28 Feet, 28 Feet &gt; and &lt;= 32 Feet, 32 Feet &gt; and &lt;= 36 Feet, Greater than 36 Feet</t>
@@ -431,7 +431,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -442,6 +442,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF2CC"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -492,7 +498,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -597,548 +603,540 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="80.9444444444445"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="59.6777777777778"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="92.0148148148148"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.4"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="67.5185185185185"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.7"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>8</v>
-      </c>
       <c r="E6" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>8</v>
-      </c>
       <c r="E19" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="E27" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="F30" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1158,12 +1156,12 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M11" activeCellId="0" sqref="M11"/>
+      <selection pane="topLeft" activeCell="G46" activeCellId="0" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1171,27 +1169,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1218,8 +1216,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.6185185185185"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="70.8481481481482"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1227,27 +1225,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1274,13 +1272,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.1703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="11.662962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B1" s="5" t="n">
         <v>1</v>
@@ -1318,13 +1316,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -1339,16 +1337,16 @@
         <v>4</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -1362,19 +1360,19 @@
         <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -1387,22 +1385,22 @@
         <v>6</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -1414,25 +1412,25 @@
         <v>7</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
@@ -1443,28 +1441,28 @@
         <v>8</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
@@ -1474,67 +1472,67 @@
         <v>9</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="J9" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>95</v>
-      </c>
       <c r="K9" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1556,33 +1554,33 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="102.207407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="115.925925925926"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>101</v>
+        <v>56</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>102</v>
@@ -1591,12 +1589,12 @@
         <v>103</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>104</v>
@@ -1605,12 +1603,12 @@
         <v>103</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>105</v>
@@ -1619,12 +1617,12 @@
         <v>103</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>106</v>
@@ -1633,7 +1631,7 @@
         <v>103</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1647,12 +1645,12 @@
         <v>103</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>109</v>
@@ -1661,12 +1659,12 @@
         <v>110</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>111</v>
@@ -1675,12 +1673,12 @@
         <v>103</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>112</v>
@@ -1689,12 +1687,12 @@
         <v>103</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>113</v>
@@ -1703,12 +1701,12 @@
         <v>103</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>114</v>
@@ -1717,7 +1715,7 @@
         <v>103</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1731,7 +1729,7 @@
         <v>103</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1753,14 +1751,15 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="78.1"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.7962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="98.0925925925926"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="88.4888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="66.637037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="111.222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1768,53 +1767,53 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1835,16 +1834,18 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.9185185185185"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.3"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="59.1888888888889"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.8740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.1222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="67.0296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1852,87 +1853,93 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="F3" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="E4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>64</v>
+    </row>
+    <row r="5" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1953,99 +1960,100 @@
   </sheetPr>
   <dimension ref="A1:D65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.3962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.9037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.6148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2074,9 +2082,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.4555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.2555555555556"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.3037037037037"/>
     <col collapsed="false" hidden="true" max="4" min="4" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2084,27 +2094,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2125,16 +2135,17 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="77.4148148148148"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.3"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.8185185185185"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.4777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="87.8037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.1222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="59.7777777777778"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.6148148148148"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2142,45 +2153,45 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>43</v>
+      <c r="A2" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2207,10 +2218,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.9777777777778"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.3"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.8185185185185"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.5407407407407"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.1222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="59.7777777777778"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2218,198 +2230,198 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>55</v>
+        <v>35</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>55</v>
-      </c>
       <c r="E10" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2436,8 +2448,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.8444444444444"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.3296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.3222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2445,51 +2459,51 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2516,8 +2530,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2814814814815"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.1037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2525,41 +2539,41 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>